<commit_message>
aligned columns to work with code
</commit_message>
<xml_diff>
--- a/data/orig/Shrew_data.xlsx
+++ b/data/orig/Shrew_data.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10308"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6042A731-66A5-EC4B-928D-D5E609E1C334}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE062B0-3AF0-3A4B-A5AE-9513766CCEBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27720" windowHeight="17000" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3215,7 +3215,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U494"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
@@ -14734,10 +14734,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="I1" sqref="I1:K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14749,7 +14749,7 @@
     <col min="9" max="13" width="9" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="45" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="45" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -14760,32 +14760,32 @@
         <v>1</v>
       </c>
       <c r="D1" s="13"/>
-      <c r="E1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="9" t="s">
+      <c r="I1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="M1" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="N1" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="O1" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="P1" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="Q1" s="23" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="54" t="s">
         <v>21</v>
       </c>
@@ -14795,32 +14795,32 @@
       <c r="C2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="50" t="s">
+      <c r="I2" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="17">
+      <c r="J2" s="17">
         <v>2806.3333333333335</v>
       </c>
-      <c r="G2" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="14">
+      <c r="K2" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="14">
         <v>1300</v>
       </c>
-      <c r="J2" s="14">
-        <v>0</v>
-      </c>
-      <c r="K2" s="14">
-        <v>0</v>
-      </c>
-      <c r="L2" s="14">
-        <v>0</v>
-      </c>
-      <c r="M2" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2" s="14">
+        <v>0</v>
+      </c>
+      <c r="O2" s="14">
+        <v>0</v>
+      </c>
+      <c r="P2" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="54" t="s">
         <v>21</v>
       </c>
@@ -14830,32 +14830,32 @@
       <c r="C3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="51" t="s">
+      <c r="I3" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="17">
+      <c r="J3" s="17">
         <v>2971.3333333333335</v>
       </c>
-      <c r="G3" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="14">
+      <c r="K3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" s="14">
         <v>1400</v>
       </c>
-      <c r="J3" s="14">
-        <v>0</v>
-      </c>
-      <c r="K3" s="14">
-        <v>0</v>
-      </c>
-      <c r="L3" s="14">
-        <v>0</v>
-      </c>
-      <c r="M3" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N3" s="14">
+        <v>0</v>
+      </c>
+      <c r="O3" s="14">
+        <v>0</v>
+      </c>
+      <c r="P3" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="54" t="s">
         <v>21</v>
       </c>
@@ -14865,32 +14865,32 @@
       <c r="C4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="51" t="s">
+      <c r="I4" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="17">
+      <c r="J4" s="17">
         <v>2971.3333333333335</v>
       </c>
-      <c r="G4" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="14">
+      <c r="K4" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="14">
         <v>1500</v>
       </c>
-      <c r="J4" s="14">
-        <v>0</v>
-      </c>
-      <c r="K4" s="14">
-        <v>0</v>
-      </c>
-      <c r="L4" s="14">
-        <v>0</v>
-      </c>
-      <c r="M4" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N4" s="14">
+        <v>0</v>
+      </c>
+      <c r="O4" s="14">
+        <v>0</v>
+      </c>
+      <c r="P4" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="54" t="s">
         <v>21</v>
       </c>
@@ -14900,32 +14900,32 @@
       <c r="C5" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="51" t="s">
+      <c r="I5" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="17">
+      <c r="J5" s="17">
         <v>2971.3333333333335</v>
       </c>
-      <c r="G5" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="14">
+      <c r="K5" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" s="14">
         <v>1600</v>
       </c>
-      <c r="J5" s="14">
-        <v>0</v>
-      </c>
-      <c r="K5" s="14">
-        <v>0</v>
-      </c>
-      <c r="L5" s="14">
-        <v>0</v>
-      </c>
-      <c r="M5" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N5" s="14">
+        <v>0</v>
+      </c>
+      <c r="O5" s="14">
+        <v>0</v>
+      </c>
+      <c r="P5" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="54" t="s">
         <v>21</v>
       </c>
@@ -14935,32 +14935,32 @@
       <c r="C6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="51" t="s">
+      <c r="I6" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="17">
+      <c r="J6" s="17">
         <v>2971.3333333333335</v>
       </c>
-      <c r="G6" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="14">
+      <c r="K6" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="M6" s="14">
         <v>1700</v>
       </c>
-      <c r="J6" s="14">
-        <v>0</v>
-      </c>
-      <c r="K6" s="14">
-        <v>0</v>
-      </c>
-      <c r="L6" s="14">
-        <v>0</v>
-      </c>
-      <c r="M6" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N6" s="14">
+        <v>0</v>
+      </c>
+      <c r="O6" s="14">
+        <v>0</v>
+      </c>
+      <c r="P6" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="54" t="s">
         <v>21</v>
       </c>
@@ -14970,32 +14970,32 @@
       <c r="C7" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="51" t="s">
+      <c r="I7" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="17">
+      <c r="J7" s="17">
         <v>3028.3333333333335</v>
       </c>
-      <c r="G7" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="14">
+      <c r="K7" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="M7" s="14">
         <v>1800</v>
       </c>
-      <c r="J7" s="14">
-        <v>0</v>
-      </c>
-      <c r="K7" s="14">
-        <v>0</v>
-      </c>
-      <c r="L7" s="14">
-        <v>0</v>
-      </c>
-      <c r="M7" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N7" s="14">
+        <v>0</v>
+      </c>
+      <c r="O7" s="14">
+        <v>0</v>
+      </c>
+      <c r="P7" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="54" t="s">
         <v>21</v>
       </c>
@@ -15005,32 +15005,32 @@
       <c r="C8" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="51" t="s">
+      <c r="I8" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="17">
+      <c r="J8" s="17">
         <v>3030</v>
       </c>
-      <c r="G8" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="14">
+      <c r="K8" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="M8" s="14">
         <v>1900</v>
       </c>
-      <c r="J8" s="14">
-        <v>0</v>
-      </c>
-      <c r="K8" s="14">
-        <v>0</v>
-      </c>
-      <c r="L8" s="14">
-        <v>0</v>
-      </c>
-      <c r="M8" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N8" s="14">
+        <v>0</v>
+      </c>
+      <c r="O8" s="14">
+        <v>0</v>
+      </c>
+      <c r="P8" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="54" t="s">
         <v>21</v>
       </c>
@@ -15040,32 +15040,32 @@
       <c r="C9" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="51" t="s">
+      <c r="I9" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="17">
+      <c r="J9" s="17">
         <v>3032.3333333333335</v>
       </c>
-      <c r="G9" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" s="14">
+      <c r="K9" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="M9" s="14">
         <v>2000</v>
       </c>
-      <c r="J9" s="14">
-        <v>0</v>
-      </c>
-      <c r="K9" s="14">
-        <v>0</v>
-      </c>
-      <c r="L9" s="14">
-        <v>0</v>
-      </c>
-      <c r="M9" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N9" s="14">
+        <v>0</v>
+      </c>
+      <c r="O9" s="14">
+        <v>0</v>
+      </c>
+      <c r="P9" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="54" t="s">
         <v>21</v>
       </c>
@@ -15075,32 +15075,32 @@
       <c r="C10" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="52" t="s">
+      <c r="I10" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="16">
+      <c r="J10" s="16">
         <v>3096</v>
       </c>
-      <c r="G10" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="14">
+      <c r="K10" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="M10" s="14">
         <v>2100</v>
       </c>
-      <c r="J10" s="14">
-        <v>0</v>
-      </c>
-      <c r="K10" s="14">
-        <v>0</v>
-      </c>
-      <c r="L10" s="14">
-        <v>0</v>
-      </c>
-      <c r="M10" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N10" s="14">
+        <v>0</v>
+      </c>
+      <c r="O10" s="14">
+        <v>0</v>
+      </c>
+      <c r="P10" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="54" t="s">
         <v>21</v>
       </c>
@@ -15110,32 +15110,32 @@
       <c r="C11" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="52" t="s">
+      <c r="I11" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="16">
+      <c r="J11" s="16">
         <v>3097</v>
       </c>
-      <c r="G11" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" s="14">
+      <c r="K11" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="M11" s="14">
         <v>2200</v>
       </c>
-      <c r="J11" s="14">
-        <v>0</v>
-      </c>
-      <c r="K11" s="14">
-        <v>0</v>
-      </c>
-      <c r="L11" s="14">
-        <v>0</v>
-      </c>
-      <c r="M11" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N11" s="14">
+        <v>0</v>
+      </c>
+      <c r="O11" s="14">
+        <v>0</v>
+      </c>
+      <c r="P11" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="54" t="s">
         <v>21</v>
       </c>
@@ -15145,32 +15145,32 @@
       <c r="C12" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="52" t="s">
+      <c r="I12" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="16">
+      <c r="J12" s="16">
         <v>3102</v>
       </c>
-      <c r="G12" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" s="14">
+      <c r="K12" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="M12" s="14">
         <v>2300</v>
       </c>
-      <c r="J12" s="14">
-        <v>0</v>
-      </c>
-      <c r="K12" s="14">
-        <v>0</v>
-      </c>
-      <c r="L12" s="14">
-        <v>0</v>
-      </c>
-      <c r="M12" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N12" s="14">
+        <v>0</v>
+      </c>
+      <c r="O12" s="14">
+        <v>0</v>
+      </c>
+      <c r="P12" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="54" t="s">
         <v>21</v>
       </c>
@@ -15180,32 +15180,32 @@
       <c r="C13" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="52" t="s">
+      <c r="I13" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="16">
+      <c r="J13" s="16">
         <v>3126</v>
       </c>
-      <c r="G13" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" s="14">
+      <c r="K13" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="M13" s="14">
         <v>2400</v>
       </c>
-      <c r="J13" s="14">
-        <v>0</v>
-      </c>
-      <c r="K13" s="14">
-        <v>0</v>
-      </c>
-      <c r="L13" s="14">
-        <v>0</v>
-      </c>
-      <c r="M13" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N13" s="14">
+        <v>0</v>
+      </c>
+      <c r="O13" s="14">
+        <v>0</v>
+      </c>
+      <c r="P13" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="54" t="s">
         <v>21</v>
       </c>
@@ -15215,32 +15215,32 @@
       <c r="C14" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="53" t="s">
+      <c r="I14" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="18">
+      <c r="J14" s="18">
         <v>3320</v>
       </c>
-      <c r="G14" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" s="14">
+      <c r="K14" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="M14" s="14">
         <v>2500</v>
       </c>
-      <c r="J14" s="14">
-        <v>0</v>
-      </c>
-      <c r="K14" s="14">
-        <v>0</v>
-      </c>
-      <c r="L14" s="14">
-        <v>0</v>
-      </c>
-      <c r="M14" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N14" s="14">
+        <v>0</v>
+      </c>
+      <c r="O14" s="14">
+        <v>0</v>
+      </c>
+      <c r="P14" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="54" t="s">
         <v>21</v>
       </c>
@@ -15250,32 +15250,32 @@
       <c r="C15" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="53" t="s">
+      <c r="I15" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="18">
+      <c r="J15" s="18">
         <v>3331</v>
       </c>
-      <c r="G15" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I15" s="14">
+      <c r="K15" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="M15" s="14">
         <v>2600</v>
       </c>
-      <c r="J15" s="14">
-        <v>0</v>
-      </c>
-      <c r="K15" s="14">
-        <v>14</v>
-      </c>
-      <c r="L15" s="14">
-        <v>0</v>
-      </c>
-      <c r="M15" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N15" s="14">
+        <v>0</v>
+      </c>
+      <c r="O15" s="14">
+        <v>14</v>
+      </c>
+      <c r="P15" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="54" t="s">
         <v>21</v>
       </c>
@@ -15285,32 +15285,32 @@
       <c r="C16" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="52" t="s">
+      <c r="I16" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="16">
+      <c r="J16" s="16">
         <v>3442</v>
       </c>
-      <c r="G16" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I16" s="14">
+      <c r="K16" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="M16" s="14">
         <v>2700</v>
       </c>
-      <c r="J16" s="14">
-        <v>0</v>
-      </c>
-      <c r="K16" s="14">
-        <v>0</v>
-      </c>
-      <c r="L16" s="14">
-        <v>0</v>
-      </c>
-      <c r="M16" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N16" s="14">
+        <v>0</v>
+      </c>
+      <c r="O16" s="14">
+        <v>0</v>
+      </c>
+      <c r="P16" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="54" t="s">
         <v>21</v>
       </c>
@@ -15320,32 +15320,32 @@
       <c r="C17" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="52" t="s">
+      <c r="I17" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="16">
+      <c r="J17" s="16">
         <v>3447</v>
       </c>
-      <c r="G17" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I17" s="14">
+      <c r="K17" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="M17" s="14">
         <v>2800</v>
       </c>
-      <c r="J17" s="14">
-        <v>0</v>
-      </c>
-      <c r="K17" s="14">
-        <v>0</v>
-      </c>
-      <c r="L17" s="14">
-        <v>0</v>
-      </c>
-      <c r="M17" s="14">
+      <c r="N17" s="14">
+        <v>0</v>
+      </c>
+      <c r="O17" s="14">
+        <v>0</v>
+      </c>
+      <c r="P17" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="54" t="s">
         <v>21</v>
       </c>
@@ -15355,32 +15355,32 @@
       <c r="C18" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="I18" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F18" s="18">
+      <c r="J18" s="18">
         <v>2926.08</v>
       </c>
-      <c r="G18" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I18" s="14">
+      <c r="K18" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="M18" s="14">
         <v>2900</v>
       </c>
-      <c r="J18" s="14">
+      <c r="N18" s="14">
         <v>2</v>
       </c>
-      <c r="K18" s="14">
+      <c r="O18" s="14">
         <v>8</v>
       </c>
-      <c r="L18" s="14">
+      <c r="P18" s="14">
         <v>1</v>
       </c>
-      <c r="M18" s="14">
+      <c r="Q18" s="14">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="54" t="s">
         <v>21</v>
       </c>
@@ -15390,32 +15390,32 @@
       <c r="C19" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="I19" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F19" s="18">
+      <c r="J19" s="18">
         <v>3063.2400000000002</v>
       </c>
-      <c r="G19" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I19" s="14">
+      <c r="K19" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="M19" s="14">
         <v>3000</v>
       </c>
-      <c r="J19" s="14">
+      <c r="N19" s="14">
         <v>1</v>
       </c>
-      <c r="K19" s="14">
-        <v>0</v>
-      </c>
-      <c r="L19" s="14">
-        <v>3</v>
-      </c>
-      <c r="M19" s="14">
+      <c r="O19" s="14">
+        <v>0</v>
+      </c>
+      <c r="P19" s="14">
+        <v>3</v>
+      </c>
+      <c r="Q19" s="14">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="54" t="s">
         <v>21</v>
       </c>
@@ -15425,32 +15425,32 @@
       <c r="C20" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="I20" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="18">
+      <c r="J20" s="18">
         <v>3063.2400000000002</v>
       </c>
-      <c r="G20" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I20" s="14">
+      <c r="K20" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="M20" s="14">
         <v>3100</v>
       </c>
-      <c r="J20" s="14">
-        <v>0</v>
-      </c>
-      <c r="K20" s="14">
-        <v>0</v>
-      </c>
-      <c r="L20" s="14">
+      <c r="N20" s="14">
+        <v>0</v>
+      </c>
+      <c r="O20" s="14">
+        <v>0</v>
+      </c>
+      <c r="P20" s="14">
         <v>2</v>
       </c>
-      <c r="M20" s="14">
+      <c r="Q20" s="14">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="54" t="s">
         <v>21</v>
       </c>
@@ -15460,32 +15460,32 @@
       <c r="C21" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="I21" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F21" s="18">
+      <c r="J21" s="18">
         <v>3063.2400000000002</v>
       </c>
-      <c r="G21" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I21" s="14">
+      <c r="K21" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="M21" s="14">
         <v>3200</v>
       </c>
-      <c r="J21" s="14">
-        <v>3</v>
-      </c>
-      <c r="K21" s="14">
-        <v>0</v>
-      </c>
-      <c r="L21" s="14">
-        <v>0</v>
-      </c>
-      <c r="M21" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N21" s="14">
+        <v>3</v>
+      </c>
+      <c r="O21" s="14">
+        <v>0</v>
+      </c>
+      <c r="P21" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="54" t="s">
         <v>21</v>
       </c>
@@ -15495,32 +15495,32 @@
       <c r="C22" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="I22" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F22" s="18">
+      <c r="J22" s="18">
         <v>3389.3760000000002</v>
       </c>
-      <c r="G22" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I22" s="14">
+      <c r="K22" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="M22" s="14">
         <v>3300</v>
       </c>
-      <c r="J22" s="14">
-        <v>0</v>
-      </c>
-      <c r="K22" s="14">
-        <v>0</v>
-      </c>
-      <c r="L22" s="14">
+      <c r="N22" s="14">
+        <v>0</v>
+      </c>
+      <c r="O22" s="14">
+        <v>0</v>
+      </c>
+      <c r="P22" s="14">
         <v>2</v>
       </c>
-      <c r="M22" s="14">
+      <c r="Q22" s="14">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="54" t="s">
         <v>21</v>
       </c>
@@ -15530,32 +15530,32 @@
       <c r="C23" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="I23" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F23" s="18">
+      <c r="J23" s="18">
         <v>3389.3760000000002</v>
       </c>
-      <c r="G23" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I23" s="14">
+      <c r="K23" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="M23" s="14">
         <v>3400</v>
       </c>
-      <c r="J23" s="14">
-        <v>0</v>
-      </c>
-      <c r="K23" s="14">
-        <v>0</v>
-      </c>
-      <c r="L23" s="14">
+      <c r="N23" s="14">
+        <v>0</v>
+      </c>
+      <c r="O23" s="14">
+        <v>0</v>
+      </c>
+      <c r="P23" s="14">
         <v>1</v>
       </c>
-      <c r="M23" s="14">
+      <c r="Q23" s="14">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="48" t="s">
         <v>32</v>
       </c>
@@ -15565,32 +15565,32 @@
       <c r="C24" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="I24" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F24" s="18">
+      <c r="J24" s="18">
         <v>3108.96</v>
       </c>
-      <c r="G24" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I24" s="14">
+      <c r="K24" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="M24" s="14">
         <v>3500</v>
       </c>
-      <c r="J24" s="14">
-        <v>0</v>
-      </c>
-      <c r="K24" s="14">
-        <v>0</v>
-      </c>
-      <c r="L24" s="14">
-        <v>0</v>
-      </c>
-      <c r="M24" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N24" s="14">
+        <v>0</v>
+      </c>
+      <c r="O24" s="14">
+        <v>0</v>
+      </c>
+      <c r="P24" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="13" t="s">
         <v>29</v>
       </c>
@@ -15600,32 +15600,32 @@
       <c r="C25" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="I25" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F25" s="18">
+      <c r="J25" s="18">
         <v>3108.96</v>
       </c>
-      <c r="G25" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I25" s="14">
+      <c r="K25" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="M25" s="14">
         <v>3600</v>
       </c>
-      <c r="J25" s="14">
-        <v>0</v>
-      </c>
-      <c r="K25" s="14">
-        <v>0</v>
-      </c>
-      <c r="L25" s="14">
-        <v>0</v>
-      </c>
-      <c r="M25" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N25" s="14">
+        <v>0</v>
+      </c>
+      <c r="O25" s="14">
+        <v>0</v>
+      </c>
+      <c r="P25" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="13" t="s">
         <v>29</v>
       </c>
@@ -15635,32 +15635,32 @@
       <c r="C26" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E26" s="13" t="s">
+      <c r="I26" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F26" s="18">
+      <c r="J26" s="18">
         <v>3407.6640000000002</v>
       </c>
-      <c r="G26" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I26" s="14">
+      <c r="K26" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="M26" s="14">
         <v>3700</v>
       </c>
-      <c r="J26" s="14">
-        <v>0</v>
-      </c>
-      <c r="K26" s="14">
-        <v>0</v>
-      </c>
-      <c r="L26" s="14">
-        <v>0</v>
-      </c>
-      <c r="M26" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N26" s="14">
+        <v>0</v>
+      </c>
+      <c r="O26" s="14">
+        <v>0</v>
+      </c>
+      <c r="P26" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="13" t="s">
         <v>29</v>
       </c>
@@ -15670,23 +15670,23 @@
       <c r="C27" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="I27" s="14">
+      <c r="M27" s="14">
         <v>3800</v>
       </c>
-      <c r="J27" s="14">
-        <v>0</v>
-      </c>
-      <c r="K27" s="14">
-        <v>0</v>
-      </c>
-      <c r="L27" s="14">
-        <v>0</v>
-      </c>
-      <c r="M27" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N27" s="14">
+        <v>0</v>
+      </c>
+      <c r="O27" s="14">
+        <v>0</v>
+      </c>
+      <c r="P27" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="13" t="s">
         <v>29</v>
       </c>
@@ -15696,23 +15696,23 @@
       <c r="C28" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="I28" s="14">
+      <c r="M28" s="14">
         <v>3900</v>
       </c>
-      <c r="J28" s="14">
-        <v>0</v>
-      </c>
-      <c r="K28" s="14">
-        <v>0</v>
-      </c>
-      <c r="L28" s="14">
-        <v>0</v>
-      </c>
-      <c r="M28" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N28" s="14">
+        <v>0</v>
+      </c>
+      <c r="O28" s="14">
+        <v>0</v>
+      </c>
+      <c r="P28" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="13" t="s">
         <v>29</v>
       </c>
@@ -15722,53 +15722,53 @@
       <c r="C29" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="I29" s="14">
+      <c r="M29" s="14">
         <v>4000</v>
       </c>
-      <c r="J29" s="14">
-        <v>0</v>
-      </c>
-      <c r="K29" s="14">
-        <v>0</v>
-      </c>
-      <c r="L29" s="14">
-        <v>0</v>
-      </c>
-      <c r="M29" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="I30" s="14">
+      <c r="N29" s="14">
+        <v>0</v>
+      </c>
+      <c r="O29" s="14">
+        <v>0</v>
+      </c>
+      <c r="P29" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="M30" s="14">
         <v>4100</v>
       </c>
-      <c r="J30" s="14">
-        <v>0</v>
-      </c>
-      <c r="K30" s="14">
-        <v>0</v>
-      </c>
-      <c r="L30" s="14">
-        <v>0</v>
-      </c>
-      <c r="M30" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="I31" s="14">
+      <c r="N30" s="14">
+        <v>0</v>
+      </c>
+      <c r="O30" s="14">
+        <v>0</v>
+      </c>
+      <c r="P30" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="M31" s="14">
         <v>4200</v>
       </c>
-      <c r="J31" s="14">
-        <v>0</v>
-      </c>
-      <c r="K31" s="14">
-        <v>0</v>
-      </c>
-      <c r="L31" s="14">
-        <v>0</v>
-      </c>
-      <c r="M31" s="14">
+      <c r="N31" s="14">
+        <v>0</v>
+      </c>
+      <c r="O31" s="14">
+        <v>0</v>
+      </c>
+      <c r="P31" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="14">
         <v>0</v>
       </c>
     </row>
@@ -17271,7 +17271,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="E4:G11">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E4:G11">
     <sortCondition ref="F4:F11"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17282,7 +17282,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Y1188"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
@@ -33992,7 +33992,7 @@
       <c r="C1188" s="13"/>
     </row>
   </sheetData>
-  <sortState ref="I97:K239">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I97:K239">
     <sortCondition ref="J97:J239"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>